<commit_message>
Models error tracking and LLM-sugested fixes summary
</commit_message>
<xml_diff>
--- a/error tracking.xlsx
+++ b/error tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSc\Jobs\AnkiLab\Projects\LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB6E0DA-91D9-436A-A04B-F6D83187B092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBFA178-CAC4-463A-80E9-7DE1755C0DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="114">
   <si>
     <t>model</t>
   </si>
@@ -264,9 +264,6 @@
     <t xml:space="preserve"> ______</t>
   </si>
   <si>
-    <t>Gemini</t>
-  </si>
-  <si>
     <t xml:space="preserve">NameError: name 'time' is not defined
 </t>
   </si>
@@ -600,6 +597,806 @@
   <si>
     <t>Claude
  3.5 Sonnet</t>
+  </si>
+  <si>
+    <t>#Errors</t>
+  </si>
+  <si>
+    <t>LLAMA 3.1 405B</t>
+  </si>
+  <si>
+    <t>train_size = int(0.8 * len(dataset))
+val_size = int(0.1 * len(dataset))
+test_size = len(dataset) - train_size - val_size
+train_dataset, val_dataset, test_dataset = torch.utils.data.random_split(dataset, [train_size, val_size, test_size])</t>
+  </si>
+  <si>
+    <t>import torch.nn.functional as F</t>
+  </si>
+  <si>
+    <t>Unresolved reference 'os'</t>
+  </si>
+  <si>
+    <t>import os</t>
+  </si>
+  <si>
+    <t>Unresolved reference 'np'</t>
+  </si>
+  <si>
+    <t>import numpy as np</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> modify the __getitem__ method of the BinarySegmentationDataset class to return tensors instead of PIL Image objects. </t>
+  </si>
+  <si>
+    <t>ensure that all images are resized to the same size before they are fed into the network.
+adding a transforms.Resize transformation to the transform variable in the BinarySegmentationDataset class.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move the model to the GPU before training. </t>
+  </si>
+  <si>
+    <t>ensure that the output of the model is the same size as the original image size. 
+adding upsampling or transposed convolutional layers to the model to increase the output size.</t>
+  </si>
+  <si>
+    <t>ensure that the output tensor and the mask tensor have the same size. 
+resizing the mask tensor to match the size of the output tensor. F interpolate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The error message indicates that the next(iter(loader)) line is expecting three values (images, masks, and outputs), but it's only getting two.
+ modify the visualize_predictions function to only expect two values from the DataLoader. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ValueError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Sum of input lengths does not equal the length of the input dataset!
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>TypeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: default_collate: batch must contain tensors, numpy arrays, numbers, dicts or lists; found &lt;class 'PIL.Image.Image'&gt;
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    return torch.stack(batch, 0, out=out)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: stack expects each tensor to be equal size, but got [1, 256, 256] at entry 0 and [1, 320, 256] at entry 2
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Input type (torch.cuda.FloatTensor) and weight type (torch.FloatTensor) should be the same
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ValueError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: Using a target size (torch.Size([32, 1, 256, 256])) that is different to the input size (torch.Size([32, 1, 240, 240])) is deprecated. Please ensure they have the same size.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ValueError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Using a target size (torch.Size([32, 1, 256, 256])) that is different to the input size (torch.Size([32, 1, 240, 240])) is deprecated. Please ensure they have the same size.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    intersection = (outputs * masks).sum()
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: The size of tensor a (240) must match the size of tensor b (256) at non-singleton dimension 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">images, masks, outputs = next(iter(loader))
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ValueError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: not enough values to unpack (expected 3, got 2)
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    masks = F.interpolate(masks, size=outputs.shape[2:], mode='nearest')
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NameError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: name 'F' is not defined</t>
+    </r>
+  </si>
+  <si>
+    <t>from torchvision import transforms</t>
+  </si>
+  <si>
+    <t>Unresolved reference 'nn'</t>
+  </si>
+  <si>
+    <t>Unresolved reference 'optim'</t>
+  </si>
+  <si>
+    <t>import torch.optim as optim</t>
+  </si>
+  <si>
+    <t>Unresolved reference 'device'</t>
+  </si>
+  <si>
+    <t>device = torch.device("cuda" if torch.cuda.is_available() else "cpu")</t>
+  </si>
+  <si>
+    <t>Microsoft Bing
+ Copilot</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    dataset = SegmentationDataset(image_dir, transform=transforms.ToTensor())
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NameError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: name 'transforms' is not defined
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> ensure that all images and masks in your dataset have the same size. 
+ resizing them during the transformation process</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 
+    enc1 = self.encoder0
+  File "C:\Users\qy44lyfe\.conda\envs\Swallowenv\lib\site-packages\torch\nn\modules\module.py", line 1688, in __getattr__
+    raise AttributeError(f"'{type(self).__name__}' object has no attribute '{name}'")
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>AttributeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: 'UNet' object has no attribute 'encoder0'. Did you mean: 'encoder'?
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">line 174, in collate_tensor_fn
+    return torch.stack(batch, 0, out=out)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: stack expects each tensor to be equal size, but got [1, 512, 256] at entry 0 and [1, 320, 256] at entry </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> using the layers defined in your encoder and decoder sequences.</t>
+  </si>
+  <si>
+    <t>Gemini 1.5 Pro</t>
+  </si>
+  <si>
+    <t>Unresolved reference 'F'</t>
+  </si>
+  <si>
+    <t>You need to move your model to the GPU as well.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+    optimizer = optim.Adam(model.parameters(), lr=learning_rate)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NameError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: name 'optim' is not defined</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> line 456, in _conv_forward
+    return F.conv2d(input, weight, bias, self.stride,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: Given groups=1, weight of size [512, 1024, 3, 3], expected input[2, 512, 16, 16] to have 1024 channels, but got 512 channels instead</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> in your upconv_block and how you're using it in the decoder part of the forward method. You're concatenating the encoder output (e4, e3, etc.) with the decoder output (d4, d3, etc.) before passing the result through the convolutional layers in the upconv_block. The convolutional layers in upconv_block are expecting the input to have in_c channels (1024 in the case of dec4), 
+but after the concatenation, the number of channels becomes in_c * 2 
+(because you concatenated along the channel dimension).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+    d4 = torch.cat((e4, d4), dim=1)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: Sizes of tensors must match except in dimension 1. Expected size 16 but got size 32 for tensor number 1 in the list.</t>
+    </r>
+  </si>
+  <si>
+    <t>The most likely cause is an incorrect padding setting in your convolutional layers or transposed convolutional layers.
+ In a U-Net, you need to ensure that the spatial dimensions of the encoder feature maps align with the upsampled feature maps from the decoder.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">d4 = torch.cat((e4, d4), dim=1)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Sizes of tensors must match except in dimension 1. Expected size 16 but got size 32 for tensor number 1 in the list.
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> The transposed convolution in the upconv_block doubles the spatial dimensions, so d4 will be 32x32 while e4 is 16x16.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">return F.conv2d(input, weight, bias, self.stride,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Input type (torch.cuda.FloatTensor) and weight type (torch.FloatTensor) should be the same
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> line 456, in _conv_forward
+    return F.conv2d(input, weight, bias, self.stride,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Input type (torch.cuda.FloatTensor) and weight type (torch.FloatTensor) should be the same
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> I assigned the methods _make_conv_block and _make_conv_block_no_pooling to self.conv_block and self.conv_block_no_pooling, respectively, 
+instead of calling the methods to create the actual nn.Sequential blocks.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ValueError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Using a target size (torch.Size([8, 1, 256, 256])) that is different to the input size (torch.Size([8, 1, 128, 128])) is deprecated. Please ensure they have the same size.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>The simplest solution is to resize your target masks to match the output size of the U-Net. You can do this within your training loop: 
+resized_masks = F.interpolate(masks, size=outputs.shape[2:], mode='nearest')</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">line 266, in backward
+Variable._execution_engine.run_backward( # Calls into the C++ engine to run the backward pass
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: cuDNN error: CUDNN_STATUS_MAPPING_ERROR
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ensure you have a sigmoid activation function at the very end of your U-Net model to produce output values between 0 and 1.
+ This is crucial for binary cross-entropy loss. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ValueError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Using a target size (torch.Size([8, 1, 256, 256])) that is different to the input size (torch.Size([8, 1, 128, 128])) is deprecated. Please ensure they have the same size.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>you also need to ensure the masks are resized during validation as well. 
+The error is occurring in your validate function because the output of the model and the masks have different sizes.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+    total_dice += dice.item()
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>AttributeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: 'float' object has no attribute 'item'
+</t>
+    </r>
+  </si>
+  <si>
+    <t>The error AttributeError: 'float' object has no attribute 'item' occurs because the dice_coeff function is already returning a single float value 
+(the average Dice coefficient across the batch). You're then trying to call .item() on this float, which is not necessary.</t>
+  </si>
+  <si>
+    <t>Use Tensor.cpu() to copy the tensor to host memory first arises because you're trying to create a Pandas DataFrame directly from a tensor that resides on the GPU. 
+Pandas DataFrames require data to be in CPU memory (host memory).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">line 1064, in __array__
+    return self.numpy().astype(dtype, copy=False)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>TypeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: can't convert cuda:0 device type tensor to numpy. Use Tensor.cpu() to copy the tensor to host memory first.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">line 1064, in array
+return self.numpy().astype(dtype, copy=False)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>TypeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: can't convert cuda:0 device type tensor to numpy. Use Tensor.cpu() to copy the tensor to host memory first.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> I missed applying the same logic to val_loss.
+ val_loss also needs to be moved to the CPU before being appended to the list.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  line 105, in &lt;module&gt;
+    val_losses.append(val_loss.cpu().item())
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>AttributeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: 'float' object has no attribute 'cpu'
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  line 88, in test
+    dice = dice_coeff(outputs, masks)
+ line 24, in dice_coeff
+    intersection = (m1 * m2).sum()
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RuntimeError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: The size of tensor a (16384) must match the size of tensor b (65536) at non-singleton dimension 1
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Interpolation: I've added outputs = F.interpolate(outputs, size=masks.shape[2:], mode='bilinear', align_corners=False) before the thresholding operation. This line uses bilinear interpolation to resize the outputs tensor to match the spatial dimensions (height and width) of the masks tensor. align_corners=False is generally recommended for better accuracy. 
+You can also use 'nearest' mode for interpolation if you prefer, but bilinear is often better for smoother results.
+Thresholding After Resizing: The thresholding operation outputs = (outputs &gt; 0.5).float() is now applied after resizing. This ensures that you are comparing masks of the same size.
+dice.cpu().item() in loop.set_postfix: I've added .cpu().item() to the dice score in the loop.set_postfix to avoid potential CUDA-related errors.
+avg_dice.cpu().item() at the end: The final avg_dice is also moved to the CPU before being returned as a standard Python float.</t>
+  </si>
+  <si>
+    <t>float' object has no attribute 'cpu' arises because val_loss is already a Python float, not a tensor. The .cpu() method is only applicable to tensors.
+ The issue is likely stemming from how you're calculating and accumulating val_loss in your validate function.</t>
+  </si>
+  <si>
+    <t>Gemini 1.5 Flash</t>
   </si>
 </sst>
 </file>
@@ -636,7 +1433,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,6 +1482,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -721,19 +1530,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -782,19 +1578,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -812,9 +1595,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -828,7 +1631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -845,20 +1648,50 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -875,86 +1708,137 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -964,6 +1848,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FFFF"/>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFEDB5F1"/>
       <color rgb="FFD553DF"/>
       <color rgb="FFFF33CC"/>
@@ -1243,283 +2129,669 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="93.6328125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="58.90625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="15.08984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="69" customWidth="1"/>
+    <col min="3" max="3" width="93.6328125" style="55" customWidth="1"/>
+    <col min="4" max="4" width="58.90625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="31" customFormat="1" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="23" t="s">
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A3" s="22"/>
+      <c r="B3" s="57">
+        <v>4</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A4" s="22"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="10" customFormat="1" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="12"/>
-      <c r="B5" s="24" t="s">
+    <row r="5" spans="1:4" s="9" customFormat="1" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="22"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="5" customFormat="1" ht="52.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="52.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="58"/>
+      <c r="C6" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="5" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
-      <c r="B7" s="25" t="s">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A7" s="24"/>
+      <c r="B7" s="59">
+        <v>3</v>
+      </c>
+      <c r="C7" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="22" customFormat="1" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="14"/>
-      <c r="B8" s="26" t="s">
+    <row r="8" spans="1:4" s="11" customFormat="1" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="24"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="D8" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="18" customFormat="1" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:4" s="10" customFormat="1" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="60"/>
+      <c r="C9" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="18" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-    </row>
-    <row r="11" spans="1:3" s="38" customFormat="1" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-    </row>
-    <row r="12" spans="1:3" s="30" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+    <row r="10" spans="1:4" s="10" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="26"/>
+      <c r="B10" s="61">
+        <v>0</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" s="16" customFormat="1" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="26"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="34"/>
+    </row>
+    <row r="12" spans="1:4" s="12" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A12" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="62"/>
+      <c r="C12" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="D12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="30" t="s">
+    </row>
+    <row r="13" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="20"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="31" t="s">
+    <row r="14" spans="1:4" s="12" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A14" s="20"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="20"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="12" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A16" s="20"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="12" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A17" s="20"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="12" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A18" s="20"/>
+      <c r="B18" s="62">
+        <v>8</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="12" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A19" s="20"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="12" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A20" s="20"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="20"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="52"/>
+    </row>
+    <row r="22" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="20"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="52"/>
+    </row>
+    <row r="23" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="20"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="52"/>
+    </row>
+    <row r="24" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="20"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="52"/>
+    </row>
+    <row r="25" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="20"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="52"/>
+    </row>
+    <row r="26" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="20"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="52"/>
+    </row>
+    <row r="27" spans="1:4" s="15" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A27" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="63"/>
+      <c r="C27" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="15" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A28" s="20"/>
+      <c r="B28" s="64">
+        <v>4</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="15" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A29" s="20"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="15" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A30" s="20"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="18" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="65">
+        <v>0</v>
+      </c>
+      <c r="C31" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="30" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="28"/>
-      <c r="B15" s="31" t="s">
+      <c r="D31" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
-      <c r="B16" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
-      <c r="B17" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="30" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
-      <c r="B18" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="30" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
-      <c r="B19" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="30" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="33"/>
-    </row>
-    <row r="22" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="33"/>
-    </row>
-    <row r="23" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="33"/>
-    </row>
-    <row r="24" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="33"/>
-    </row>
-    <row r="25" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="33"/>
-    </row>
-    <row r="26" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="33"/>
-    </row>
-    <row r="27" spans="1:3" s="35" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A27" s="36" t="s">
+    </row>
+    <row r="32" spans="1:4" s="28" customFormat="1" ht="78" x14ac:dyDescent="0.35">
+      <c r="A32" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="66"/>
+      <c r="C32" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="28" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A33" s="24"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="28" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A34" s="24"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="28" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A35" s="24"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="28" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A36" s="24"/>
+      <c r="B36" s="66">
+        <v>11</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="28" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A37" s="24"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="28" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A38" s="24"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="24"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="24"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="28" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A41" s="24"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="28" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A42" s="24"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="27"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="54"/>
+    </row>
+    <row r="44" spans="1:4" s="38" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A44" s="36"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="36"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="35" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A28" s="37"/>
-      <c r="B28" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="35" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A29" s="37"/>
-      <c r="B29" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="35" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A30" s="37"/>
-      <c r="B30" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="42" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="41" t="s">
-        <v>48</v>
+    </row>
+    <row r="46" spans="1:4" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="36"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="36"/>
+      <c r="B47" s="67"/>
+      <c r="C47" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="38" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A48" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="67">
+        <v>6</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="38" customFormat="1" ht="91" x14ac:dyDescent="0.35">
+      <c r="A49" s="36"/>
+      <c r="B49" s="67"/>
+      <c r="C49" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="43" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A50" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="68"/>
+      <c r="C50" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="43" customFormat="1" ht="91" x14ac:dyDescent="0.35">
+      <c r="A51" s="44"/>
+      <c r="B51" s="68"/>
+      <c r="C51" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="43" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A52" s="44"/>
+      <c r="B52" s="68"/>
+      <c r="C52" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="43" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A53" s="44"/>
+      <c r="B53" s="68"/>
+      <c r="C53" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="43" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="44"/>
+      <c r="B54" s="68"/>
+      <c r="C54" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="43" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A55" s="44"/>
+      <c r="B55" s="68"/>
+      <c r="C55" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="43" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A56" s="44"/>
+      <c r="B56" s="68"/>
+      <c r="C56" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="43" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A57" s="44"/>
+      <c r="B57" s="68"/>
+      <c r="C57" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="43" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A58" s="44"/>
+      <c r="B58" s="68">
+        <v>15</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="43" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A59" s="44"/>
+      <c r="B59" s="68"/>
+      <c r="C59" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="43" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A60" s="44"/>
+      <c r="B60" s="68"/>
+      <c r="C60" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" s="41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="43" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A61" s="44"/>
+      <c r="B61" s="68"/>
+      <c r="C61" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" s="43" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A62" s="44"/>
+      <c r="B62" s="68"/>
+      <c r="C62" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" s="41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="43" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A63" s="44"/>
+      <c r="B63" s="68"/>
+      <c r="C63" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" s="45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" s="43" customFormat="1" ht="182" x14ac:dyDescent="0.35">
+      <c r="A64" s="44"/>
+      <c r="B64" s="68"/>
+      <c r="C64" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="41" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C9:C11"/>
+  <mergeCells count="9">
+    <mergeCell ref="A32:A42"/>
+    <mergeCell ref="A12:A26"/>
+    <mergeCell ref="A50:A64"/>
+    <mergeCell ref="D9:D11"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>